<commit_message>
Fix name and date
</commit_message>
<xml_diff>
--- a/hardware/keyboard-classic/classic-ascii-keycaps.xlsx
+++ b/hardware/keyboard-classic/classic-ascii-keycaps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/vsrc/unified_retro_keyboard/hardware/keyboard-classic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C97425C-DC17-8944-B24E-4482B10DBE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7C3764-26B4-BE43-AED0-143A7458676D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19640" yWindow="5360" windowWidth="41160" windowHeight="30100" xr2:uid="{5947D8F6-B0FF-824B-90A6-066CA128251B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="127">
   <si>
     <t>Size</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Order specifications for Signature Plastics keycaps</t>
   </si>
   <si>
-    <t>HP 9830a key set</t>
-  </si>
-  <si>
     <t>TBT</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>RUN</t>
+  </si>
+  <si>
+    <t>Classic Keycap set</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,6 +505,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -533,13 +536,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>429346</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>118324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1795419</xdr:colOff>
-      <xdr:row>108</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>197206</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -876,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76B701B-B3BE-9240-9526-A5AC01D01246}">
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,20 +900,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16" t="s">
+      <c r="A1" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17">
-        <v>44465</v>
-      </c>
-      <c r="H1" s="15"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18">
+        <v>44505</v>
+      </c>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -1018,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>4</v>
@@ -1036,17 +1039,17 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f t="shared" ref="A11:A76" si="0">A10+1</f>
+        <f t="shared" ref="A11:A77" si="0">A10+1</f>
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>53</v>
@@ -1143,8 +1146,8 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>A14+1</f>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>102</v>
@@ -1162,14 +1165,12 @@
         <v>105</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>A15+1</f>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>102</v>
@@ -1180,24 +1181,21 @@
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J17" s="1"/>
+      <c r="K17" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>102</v>
@@ -1207,6 +1205,12 @@
       </c>
       <c r="D18" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>11</v>
@@ -1219,7 +1223,7 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>102</v>
@@ -1231,7 +1235,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>105</v>
@@ -1241,7 +1245,7 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>102</v>
@@ -1253,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>105</v>
@@ -1263,7 +1267,7 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>102</v>
@@ -1275,7 +1279,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>105</v>
@@ -1285,7 +1289,7 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>102</v>
@@ -1303,48 +1307,48 @@
         <v>105</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="6" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H23" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J23" s="1"/>
+      <c r="K23" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>105</v>
@@ -1354,19 +1358,19 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>105</v>
@@ -1376,19 +1380,19 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>105</v>
@@ -1398,7 +1402,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>102</v>
@@ -1408,12 +1412,6 @@
       </c>
       <c r="D27" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>18</v>
@@ -1426,7 +1424,7 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>102</v>
@@ -1437,8 +1435,14 @@
       <c r="D28" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>105</v>
@@ -1448,7 +1452,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>102</v>
@@ -1460,7 +1464,7 @@
         <v>4</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>105</v>
@@ -1470,7 +1474,7 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>102</v>
@@ -1480,12 +1484,6 @@
       </c>
       <c r="D30" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>20</v>
@@ -1498,7 +1496,7 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>102</v>
@@ -1509,8 +1507,14 @@
       <c r="D31" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="G31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>105</v>
@@ -1520,7 +1524,7 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>102</v>
@@ -1532,7 +1536,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>105</v>
@@ -1542,7 +1546,7 @@
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>102</v>
@@ -1554,7 +1558,7 @@
         <v>4</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>105</v>
@@ -1564,7 +1568,7 @@
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>102</v>
@@ -1576,7 +1580,7 @@
         <v>4</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>105</v>
@@ -1586,7 +1590,7 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>102</v>
@@ -1598,7 +1602,7 @@
         <v>4</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>105</v>
@@ -1608,7 +1612,7 @@
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
@@ -1620,7 +1624,7 @@
         <v>4</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>105</v>
@@ -1630,7 +1634,7 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>102</v>
@@ -1642,7 +1646,7 @@
         <v>4</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>105</v>
@@ -1652,7 +1656,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>102</v>
@@ -1664,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>105</v>
@@ -1674,7 +1678,7 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>102</v>
@@ -1686,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>105</v>
@@ -1696,7 +1700,7 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>102</v>
@@ -1708,7 +1712,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>105</v>
@@ -1718,7 +1722,7 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>102</v>
@@ -1729,14 +1733,8 @@
       <c r="D41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G41" s="1">
-        <v>1</v>
+      <c r="G41" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>105</v>
@@ -1746,7 +1744,7 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>102</v>
@@ -1758,13 +1756,13 @@
         <v>4</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>105</v>
@@ -1774,7 +1772,7 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>102</v>
@@ -1786,13 +1784,13 @@
         <v>4</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G43" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>105</v>
@@ -1802,7 +1800,7 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>102</v>
@@ -1814,13 +1812,13 @@
         <v>4</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G44" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>105</v>
@@ -1830,7 +1828,7 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>102</v>
@@ -1842,13 +1840,13 @@
         <v>4</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G45" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>105</v>
@@ -1858,7 +1856,7 @@
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>102</v>
@@ -1870,13 +1868,13 @@
         <v>4</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G46" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>105</v>
@@ -1886,7 +1884,7 @@
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>102</v>
@@ -1897,27 +1895,24 @@
       <c r="D47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>97</v>
+      <c r="E47" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G47" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J47" s="1"/>
-      <c r="K47" s="6" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>102</v>
@@ -1928,24 +1923,27 @@
       <c r="D48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>37</v>
+      <c r="E48" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G48" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J48" s="1"/>
+      <c r="K48" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>102</v>
@@ -1957,13 +1955,13 @@
         <v>4</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G49" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>105</v>
@@ -1973,7 +1971,7 @@
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>102</v>
@@ -1984,8 +1982,14 @@
       <c r="D50" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="G50" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>105</v>
@@ -1995,7 +1999,7 @@
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>102</v>
@@ -2006,14 +2010,8 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>40</v>
+      <c r="G51" s="1">
+        <v>0</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>105</v>
@@ -2023,7 +2021,7 @@
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
@@ -2035,26 +2033,23 @@
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J52" s="1"/>
-      <c r="K52" s="6" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>102</v>
@@ -2066,23 +2061,26 @@
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J53" s="1"/>
+      <c r="K53" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>102</v>
@@ -2094,26 +2092,23 @@
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="K54" s="6" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>102</v>
@@ -2125,54 +2120,57 @@
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F56" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J56" s="1"/>
+      <c r="K56" s="6" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>102</v>
@@ -2184,13 +2182,13 @@
         <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>105</v>
@@ -2200,7 +2198,7 @@
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>102</v>
@@ -2212,13 +2210,13 @@
         <v>4</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>105</v>
@@ -2228,7 +2226,7 @@
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>102</v>
@@ -2240,13 +2238,13 @@
         <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>105</v>
@@ -2256,7 +2254,7 @@
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>102</v>
@@ -2267,27 +2265,24 @@
       <c r="D60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="4" t="s">
-        <v>80</v>
+      <c r="E60" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J60" s="1"/>
-      <c r="K60" s="6" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>102</v>
@@ -2299,26 +2294,26 @@
         <v>4</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>102</v>
@@ -2329,21 +2324,27 @@
       <c r="D62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="4"/>
-      <c r="I62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="E62" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J62" s="1"/>
       <c r="K62" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>102</v>
@@ -2356,19 +2357,19 @@
       </c>
       <c r="E63" s="4"/>
       <c r="I63" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J63" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>95</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>102</v>
@@ -2381,19 +2382,19 @@
       </c>
       <c r="E64" s="4"/>
       <c r="I64" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J64" s="5" t="s">
         <v>95</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>102</v>
@@ -2406,19 +2407,19 @@
       </c>
       <c r="E65" s="4"/>
       <c r="I65" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>95</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>102</v>
@@ -2429,17 +2430,21 @@
       <c r="D66" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E66" s="4"/>
       <c r="I66" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>102</v>
@@ -2451,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>53</v>
@@ -2460,7 +2465,7 @@
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>102</v>
@@ -2472,7 +2477,7 @@
         <v>4</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>53</v>
@@ -2481,7 +2486,7 @@
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>102</v>
@@ -2493,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>53</v>
@@ -2502,7 +2507,7 @@
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>102</v>
@@ -2514,7 +2519,7 @@
         <v>4</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>53</v>
@@ -2523,7 +2528,7 @@
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>102</v>
@@ -2535,17 +2540,16 @@
         <v>4</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K71" s="7"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>102</v>
@@ -2557,16 +2561,17 @@
         <v>4</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="K72" s="7"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>102</v>
@@ -2577,24 +2582,17 @@
       <c r="D73" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F73" s="1" t="s">
+      <c r="I73" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J73" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G73" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>102</v>
@@ -2606,13 +2604,13 @@
         <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>53</v>
@@ -2622,7 +2620,7 @@
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>102</v>
@@ -2634,13 +2632,13 @@
         <v>4</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>53</v>
@@ -2650,7 +2648,7 @@
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>102</v>
@@ -2662,7 +2660,7 @@
         <v>4</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>53</v>
@@ -2677,8 +2675,8 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <f t="shared" ref="A77:A83" si="1">A76+1</f>
-        <v>68</v>
+        <f t="shared" si="0"/>
+        <v>67</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>102</v>
@@ -2690,24 +2688,23 @@
         <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J77" s="1"/>
-      <c r="K77" s="7"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <f t="shared" si="1"/>
-        <v>69</v>
+        <f t="shared" ref="A78:A84" si="1">A77+1</f>
+        <v>68</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>102</v>
@@ -2716,22 +2713,27 @@
         <v>112</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K78" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="G78" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J78" s="1"/>
+      <c r="K78" s="7"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>102</v>
@@ -2749,13 +2751,13 @@
         <v>53</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>102</v>
@@ -2767,16 +2769,19 @@
         <v>51</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>53</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>102</v>
@@ -2788,87 +2793,97 @@
         <v>51</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K81" s="7"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
-      <c r="K82" s="6" t="s">
-        <v>104</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K82" s="7"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+      <c r="K83" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B84" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D83" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J83" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K83" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
+      <c r="D84" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="9"/>
-      <c r="K84" s="10"/>
+      <c r="I84" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J84" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="10"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86"/>
@@ -2902,6 +2917,17 @@
       <c r="G88"/>
       <c r="H88"/>
       <c r="I88"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>